<commit_message>
incorporate negaoctet production emissions
</commit_message>
<xml_diff>
--- a/docs/supporting/pc_emissions_model.xlsx
+++ b/docs/supporting/pc_emissions_model.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bokelley/src/methodology/docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bokelley/src/methodology/docs/supporting/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AFA9FAC-620E-274B-BF9D-A4D634762187}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5435E85D-2B3B-0241-97B9-EF9A69776314}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3660" yWindow="2660" windowWidth="27640" windowHeight="16940" activeTab="2" xr2:uid="{35CF7F97-C8CD-114B-B6E3-1E1EA0AAA903}"/>
+    <workbookView xWindow="3660" yWindow="2660" windowWidth="27640" windowHeight="16940" xr2:uid="{35CF7F97-C8CD-114B-B6E3-1E1EA0AAA903}"/>
   </bookViews>
   <sheets>
     <sheet name="PC" sheetId="1" r:id="rId1"/>
@@ -142,10 +142,10 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="5">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="_(* #,##0.000_);_(* \(#,##0.000\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="169" formatCode="#,##0.0"/>
+    <numFmt numFmtId="167" formatCode="#,##0.0"/>
+    <numFmt numFmtId="168" formatCode="_(* #,##0.0000_);_(* \(#,##0.0000\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -206,16 +206,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -532,10 +532,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D3F019F-9BA6-864D-BF85-611ACAE4DB15}">
-  <dimension ref="E9:K14"/>
+  <dimension ref="E9:K15"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -571,9 +571,8 @@
       <c r="E10" t="s">
         <v>0</v>
       </c>
-      <c r="F10" s="4">
-        <f>(218+628)/2</f>
-        <v>423</v>
+      <c r="F10" s="3">
+        <v>277</v>
       </c>
       <c r="G10" s="1">
         <f>72/194</f>
@@ -583,25 +582,24 @@
         <f>(4.6+4.8)</f>
         <v>9.3999999999999986</v>
       </c>
-      <c r="I10" s="4">
+      <c r="I10" s="3">
         <f>(59*4.6+85*4.8)/H10</f>
         <v>72.276595744680861</v>
       </c>
-      <c r="J10" s="4">
-        <v>5.5</v>
-      </c>
-      <c r="K10" s="3">
+      <c r="J10" s="3">
+        <v>6</v>
+      </c>
+      <c r="K10" s="10">
         <f>F10/J10/365/H10/3600*1000</f>
-        <v>6.2266500622665012E-3</v>
+        <v>3.7377073955331031E-3</v>
       </c>
     </row>
     <row r="11" spans="5:11" x14ac:dyDescent="0.2">
       <c r="E11" t="s">
         <v>1</v>
       </c>
-      <c r="F11" s="4">
-        <f>(281+468)/2</f>
-        <v>374.5</v>
+      <c r="F11" s="3">
+        <v>175</v>
       </c>
       <c r="G11" s="1">
         <f>122/194</f>
@@ -610,24 +608,24 @@
       <c r="H11" s="2">
         <v>6.7</v>
       </c>
-      <c r="I11" s="4">
+      <c r="I11" s="3">
         <f>(11*3+22*3.7)/6.7</f>
         <v>17.074626865671643</v>
       </c>
-      <c r="J11" s="4">
-        <v>7</v>
-      </c>
-      <c r="K11" s="3">
+      <c r="J11" s="3">
+        <v>5</v>
+      </c>
+      <c r="K11" s="10">
         <f t="shared" ref="K11:K12" si="0">F11/J11/365/H11/3600*1000</f>
-        <v>6.0769213294259309E-3</v>
+        <v>3.9755560099048138E-3</v>
       </c>
     </row>
     <row r="12" spans="5:11" x14ac:dyDescent="0.2">
       <c r="E12" t="s">
         <v>2</v>
       </c>
-      <c r="F12" s="4">
-        <v>95</v>
+      <c r="F12" s="3">
+        <v>69</v>
       </c>
       <c r="G12" s="1">
         <f>101/194</f>
@@ -636,34 +634,37 @@
       <c r="H12" s="2">
         <v>5.5</v>
       </c>
-      <c r="I12" s="4">
+      <c r="I12" s="3">
         <v>30</v>
       </c>
-      <c r="J12" s="4">
+      <c r="J12" s="3">
         <v>6.6</v>
       </c>
-      <c r="K12" s="3">
+      <c r="K12" s="10">
         <f t="shared" si="0"/>
-        <v>1.9916894138562878E-3</v>
+        <v>1.4465954690114091E-3</v>
       </c>
     </row>
     <row r="13" spans="5:11" x14ac:dyDescent="0.2">
-      <c r="F13" s="4"/>
-      <c r="K13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="K13" s="10"/>
     </row>
     <row r="14" spans="5:11" x14ac:dyDescent="0.2">
       <c r="E14" t="s">
         <v>8</v>
       </c>
-      <c r="F14" s="4"/>
-      <c r="I14" s="4">
+      <c r="F14" s="3"/>
+      <c r="I14" s="3">
         <f>SUMPRODUCT(G10:G12,I10:I12)</f>
         <v>53.180512222829705</v>
       </c>
-      <c r="K14" s="3">
+      <c r="K14" s="10">
         <f>SUMPRODUCT(G10:G12,K10:K12)</f>
-        <v>7.1694012240857566E-3</v>
-      </c>
+        <v>4.6404067425614591E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="K15" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -775,7 +776,7 @@
       <c r="F16">
         <v>20</v>
       </c>
-      <c r="G16" s="4">
+      <c r="G16" s="3">
         <f>(14*4.4+9*5.7)/(4.4+5.7)</f>
         <v>11.178217821782177</v>
       </c>
@@ -788,7 +789,7 @@
       <c r="E18" t="s">
         <v>20</v>
       </c>
-      <c r="G18" s="4">
+      <c r="G18" s="3">
         <f>SUMPRODUCT(F11:F16,G11:G16)/284</f>
         <v>87.371705480407201</v>
       </c>
@@ -802,7 +803,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DBF20CB-EC62-8543-9C04-FE3F502E9283}">
   <dimension ref="D7:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
@@ -822,7 +823,7 @@
       <c r="D8" t="s">
         <v>29</v>
       </c>
-      <c r="E8" s="10">
+      <c r="E8" s="8">
         <v>18.942</v>
       </c>
       <c r="G8" t="s">
@@ -838,10 +839,10 @@
       </c>
     </row>
     <row r="10" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="4">
         <f>0.2*E9</f>
         <v>50</v>
       </c>
@@ -850,7 +851,7 @@
       <c r="D11" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E11" s="5">
         <f>E10*E8</f>
         <v>947.1</v>
       </c>
@@ -859,7 +860,7 @@
       <c r="D13" t="s">
         <v>24</v>
       </c>
-      <c r="E13" s="7">
+      <c r="E13" s="6">
         <f>1.3*E11*1000000000/1024/1024</f>
         <v>1174192.4285888672</v>
       </c>
@@ -868,7 +869,7 @@
       <c r="D14" t="s">
         <v>25</v>
       </c>
-      <c r="E14" s="7">
+      <c r="E14" s="6">
         <f>E13*0.03</f>
         <v>35225.772857666016</v>
       </c>
@@ -877,7 +878,7 @@
       <c r="D15" t="s">
         <v>26</v>
       </c>
-      <c r="E15" s="7">
+      <c r="E15" s="6">
         <f>347*E14</f>
         <v>12223343.181610107</v>
       </c>
@@ -886,7 +887,7 @@
       <c r="D17" t="s">
         <v>27</v>
       </c>
-      <c r="E17" s="7">
+      <c r="E17" s="6">
         <f>0.000365*E11*1000000000</f>
         <v>345691500</v>
       </c>
@@ -895,7 +896,7 @@
       <c r="D19" t="s">
         <v>31</v>
       </c>
-      <c r="E19" s="8">
+      <c r="E19" s="7">
         <f>(E17+E15)/1000000*12</f>
         <v>4294.9781181793205</v>
       </c>

</xml_diff>

<commit_message>
incorporate negaoctet ademe 1.4 production emissions (#108)
* incorporate negaoctet production emissions

* add set-top box to TV emissions

* fixed unit test to account for revised device emissions values

---------

Co-authored-by: Ron Lissack <rlissack@scope3.com>
</commit_message>
<xml_diff>
--- a/docs/supporting/pc_emissions_model.xlsx
+++ b/docs/supporting/pc_emissions_model.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bokelley/src/methodology/docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bokelley/src/methodology/docs/supporting/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AFA9FAC-620E-274B-BF9D-A4D634762187}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5435E85D-2B3B-0241-97B9-EF9A69776314}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3660" yWindow="2660" windowWidth="27640" windowHeight="16940" activeTab="2" xr2:uid="{35CF7F97-C8CD-114B-B6E3-1E1EA0AAA903}"/>
+    <workbookView xWindow="3660" yWindow="2660" windowWidth="27640" windowHeight="16940" xr2:uid="{35CF7F97-C8CD-114B-B6E3-1E1EA0AAA903}"/>
   </bookViews>
   <sheets>
     <sheet name="PC" sheetId="1" r:id="rId1"/>
@@ -142,10 +142,10 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="5">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="_(* #,##0.000_);_(* \(#,##0.000\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="169" formatCode="#,##0.0"/>
+    <numFmt numFmtId="167" formatCode="#,##0.0"/>
+    <numFmt numFmtId="168" formatCode="_(* #,##0.0000_);_(* \(#,##0.0000\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -206,16 +206,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -532,10 +532,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D3F019F-9BA6-864D-BF85-611ACAE4DB15}">
-  <dimension ref="E9:K14"/>
+  <dimension ref="E9:K15"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -571,9 +571,8 @@
       <c r="E10" t="s">
         <v>0</v>
       </c>
-      <c r="F10" s="4">
-        <f>(218+628)/2</f>
-        <v>423</v>
+      <c r="F10" s="3">
+        <v>277</v>
       </c>
       <c r="G10" s="1">
         <f>72/194</f>
@@ -583,25 +582,24 @@
         <f>(4.6+4.8)</f>
         <v>9.3999999999999986</v>
       </c>
-      <c r="I10" s="4">
+      <c r="I10" s="3">
         <f>(59*4.6+85*4.8)/H10</f>
         <v>72.276595744680861</v>
       </c>
-      <c r="J10" s="4">
-        <v>5.5</v>
-      </c>
-      <c r="K10" s="3">
+      <c r="J10" s="3">
+        <v>6</v>
+      </c>
+      <c r="K10" s="10">
         <f>F10/J10/365/H10/3600*1000</f>
-        <v>6.2266500622665012E-3</v>
+        <v>3.7377073955331031E-3</v>
       </c>
     </row>
     <row r="11" spans="5:11" x14ac:dyDescent="0.2">
       <c r="E11" t="s">
         <v>1</v>
       </c>
-      <c r="F11" s="4">
-        <f>(281+468)/2</f>
-        <v>374.5</v>
+      <c r="F11" s="3">
+        <v>175</v>
       </c>
       <c r="G11" s="1">
         <f>122/194</f>
@@ -610,24 +608,24 @@
       <c r="H11" s="2">
         <v>6.7</v>
       </c>
-      <c r="I11" s="4">
+      <c r="I11" s="3">
         <f>(11*3+22*3.7)/6.7</f>
         <v>17.074626865671643</v>
       </c>
-      <c r="J11" s="4">
-        <v>7</v>
-      </c>
-      <c r="K11" s="3">
+      <c r="J11" s="3">
+        <v>5</v>
+      </c>
+      <c r="K11" s="10">
         <f t="shared" ref="K11:K12" si="0">F11/J11/365/H11/3600*1000</f>
-        <v>6.0769213294259309E-3</v>
+        <v>3.9755560099048138E-3</v>
       </c>
     </row>
     <row r="12" spans="5:11" x14ac:dyDescent="0.2">
       <c r="E12" t="s">
         <v>2</v>
       </c>
-      <c r="F12" s="4">
-        <v>95</v>
+      <c r="F12" s="3">
+        <v>69</v>
       </c>
       <c r="G12" s="1">
         <f>101/194</f>
@@ -636,34 +634,37 @@
       <c r="H12" s="2">
         <v>5.5</v>
       </c>
-      <c r="I12" s="4">
+      <c r="I12" s="3">
         <v>30</v>
       </c>
-      <c r="J12" s="4">
+      <c r="J12" s="3">
         <v>6.6</v>
       </c>
-      <c r="K12" s="3">
+      <c r="K12" s="10">
         <f t="shared" si="0"/>
-        <v>1.9916894138562878E-3</v>
+        <v>1.4465954690114091E-3</v>
       </c>
     </row>
     <row r="13" spans="5:11" x14ac:dyDescent="0.2">
-      <c r="F13" s="4"/>
-      <c r="K13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="K13" s="10"/>
     </row>
     <row r="14" spans="5:11" x14ac:dyDescent="0.2">
       <c r="E14" t="s">
         <v>8</v>
       </c>
-      <c r="F14" s="4"/>
-      <c r="I14" s="4">
+      <c r="F14" s="3"/>
+      <c r="I14" s="3">
         <f>SUMPRODUCT(G10:G12,I10:I12)</f>
         <v>53.180512222829705</v>
       </c>
-      <c r="K14" s="3">
+      <c r="K14" s="10">
         <f>SUMPRODUCT(G10:G12,K10:K12)</f>
-        <v>7.1694012240857566E-3</v>
-      </c>
+        <v>4.6404067425614591E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="K15" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -775,7 +776,7 @@
       <c r="F16">
         <v>20</v>
       </c>
-      <c r="G16" s="4">
+      <c r="G16" s="3">
         <f>(14*4.4+9*5.7)/(4.4+5.7)</f>
         <v>11.178217821782177</v>
       </c>
@@ -788,7 +789,7 @@
       <c r="E18" t="s">
         <v>20</v>
       </c>
-      <c r="G18" s="4">
+      <c r="G18" s="3">
         <f>SUMPRODUCT(F11:F16,G11:G16)/284</f>
         <v>87.371705480407201</v>
       </c>
@@ -802,7 +803,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DBF20CB-EC62-8543-9C04-FE3F502E9283}">
   <dimension ref="D7:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
@@ -822,7 +823,7 @@
       <c r="D8" t="s">
         <v>29</v>
       </c>
-      <c r="E8" s="10">
+      <c r="E8" s="8">
         <v>18.942</v>
       </c>
       <c r="G8" t="s">
@@ -838,10 +839,10 @@
       </c>
     </row>
     <row r="10" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="4">
         <f>0.2*E9</f>
         <v>50</v>
       </c>
@@ -850,7 +851,7 @@
       <c r="D11" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E11" s="5">
         <f>E10*E8</f>
         <v>947.1</v>
       </c>
@@ -859,7 +860,7 @@
       <c r="D13" t="s">
         <v>24</v>
       </c>
-      <c r="E13" s="7">
+      <c r="E13" s="6">
         <f>1.3*E11*1000000000/1024/1024</f>
         <v>1174192.4285888672</v>
       </c>
@@ -868,7 +869,7 @@
       <c r="D14" t="s">
         <v>25</v>
       </c>
-      <c r="E14" s="7">
+      <c r="E14" s="6">
         <f>E13*0.03</f>
         <v>35225.772857666016</v>
       </c>
@@ -877,7 +878,7 @@
       <c r="D15" t="s">
         <v>26</v>
       </c>
-      <c r="E15" s="7">
+      <c r="E15" s="6">
         <f>347*E14</f>
         <v>12223343.181610107</v>
       </c>
@@ -886,7 +887,7 @@
       <c r="D17" t="s">
         <v>27</v>
       </c>
-      <c r="E17" s="7">
+      <c r="E17" s="6">
         <f>0.000365*E11*1000000000</f>
         <v>345691500</v>
       </c>
@@ -895,7 +896,7 @@
       <c r="D19" t="s">
         <v>31</v>
       </c>
-      <c r="E19" s="8">
+      <c r="E19" s="7">
         <f>(E17+E15)/1000000*12</f>
         <v>4294.9781181793205</v>
       </c>

</xml_diff>

<commit_message>
add smart speaker as a device type (#141)
* add smart speaker

* add defaults

* fix default

* fix default

* run properly
</commit_message>
<xml_diff>
--- a/docs/supporting/pc_emissions_model.xlsx
+++ b/docs/supporting/pc_emissions_model.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bokelley/src/methodology/docs/supporting/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brianokelley/Documents/src/methodology/docs/supporting/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5435E85D-2B3B-0241-97B9-EF9A69776314}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D229FF5-5F36-224E-817D-0DF5AE1B4E8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3660" yWindow="2660" windowWidth="27640" windowHeight="16940" xr2:uid="{35CF7F97-C8CD-114B-B6E3-1E1EA0AAA903}"/>
+    <workbookView xWindow="3660" yWindow="2660" windowWidth="27640" windowHeight="16940" activeTab="2" xr2:uid="{35CF7F97-C8CD-114B-B6E3-1E1EA0AAA903}"/>
   </bookViews>
   <sheets>
     <sheet name="PC" sheetId="1" r:id="rId1"/>
     <sheet name="TV" sheetId="2" r:id="rId2"/>
-    <sheet name="Cookies" sheetId="3" r:id="rId3"/>
+    <sheet name="Speaker" sheetId="4" r:id="rId3"/>
+    <sheet name="Cookies" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="37">
   <si>
     <t>Desktop</t>
   </si>
@@ -134,6 +135,21 @@
   </si>
   <si>
     <t>Total annual emissions (mt CO2e)</t>
+  </si>
+  <si>
+    <t>Google Home Mini</t>
+  </si>
+  <si>
+    <t>Amazon Echo (2nd gen)</t>
+  </si>
+  <si>
+    <t>Google Home</t>
+  </si>
+  <si>
+    <t>Apple HomePod</t>
+  </si>
+  <si>
+    <t>Smart Speaker</t>
   </si>
 </sst>
 </file>
@@ -142,10 +158,10 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="5">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="0.0"/>
-    <numFmt numFmtId="166" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="167" formatCode="#,##0.0"/>
-    <numFmt numFmtId="168" formatCode="_(* #,##0.0000_);_(* \(#,##0.0000\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="#,##0.0"/>
+    <numFmt numFmtId="167" formatCode="_(* #,##0.0000_);_(* \(#,##0.0000\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -206,16 +222,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -534,7 +550,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D3F019F-9BA6-864D-BF85-611ACAE4DB15}">
   <dimension ref="E9:K15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
@@ -589,7 +605,7 @@
       <c r="J10" s="3">
         <v>6</v>
       </c>
-      <c r="K10" s="10">
+      <c r="K10" s="9">
         <f>F10/J10/365/H10/3600*1000</f>
         <v>3.7377073955331031E-3</v>
       </c>
@@ -615,7 +631,7 @@
       <c r="J11" s="3">
         <v>5</v>
       </c>
-      <c r="K11" s="10">
+      <c r="K11" s="9">
         <f t="shared" ref="K11:K12" si="0">F11/J11/365/H11/3600*1000</f>
         <v>3.9755560099048138E-3</v>
       </c>
@@ -640,14 +656,14 @@
       <c r="J12" s="3">
         <v>6.6</v>
       </c>
-      <c r="K12" s="10">
+      <c r="K12" s="9">
         <f t="shared" si="0"/>
         <v>1.4465954690114091E-3</v>
       </c>
     </row>
     <row r="13" spans="5:11" x14ac:dyDescent="0.2">
       <c r="F13" s="3"/>
-      <c r="K13" s="10"/>
+      <c r="K13" s="9"/>
     </row>
     <row r="14" spans="5:11" x14ac:dyDescent="0.2">
       <c r="E14" t="s">
@@ -658,13 +674,13 @@
         <f>SUMPRODUCT(G10:G12,I10:I12)</f>
         <v>53.180512222829705</v>
       </c>
-      <c r="K14" s="10">
+      <c r="K14" s="9">
         <f>SUMPRODUCT(G10:G12,K10:K12)</f>
         <v>4.6404067425614591E-3</v>
       </c>
     </row>
     <row r="15" spans="5:11" x14ac:dyDescent="0.2">
-      <c r="K15" s="10"/>
+      <c r="K15" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -800,6 +816,109 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D95A215D-8D33-BF44-9694-7E723B63CC15}">
+  <dimension ref="E10:H18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="5" max="5" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="10" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="E10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" t="s">
+        <v>12</v>
+      </c>
+      <c r="H10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="E11" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11">
+        <v>4</v>
+      </c>
+      <c r="G11">
+        <v>1.7</v>
+      </c>
+      <c r="H11">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="12" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="E12" t="s">
+        <v>33</v>
+      </c>
+      <c r="F12">
+        <v>35</v>
+      </c>
+      <c r="G12">
+        <v>2.4</v>
+      </c>
+      <c r="H12">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="13" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="E13" t="s">
+        <v>34</v>
+      </c>
+      <c r="F13">
+        <v>8</v>
+      </c>
+      <c r="G13">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="H13">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="14" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="E14" t="s">
+        <v>35</v>
+      </c>
+      <c r="F14">
+        <v>3</v>
+      </c>
+      <c r="G14">
+        <v>5.9</v>
+      </c>
+      <c r="H14">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="16" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="G16" s="3"/>
+    </row>
+    <row r="18" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E18" t="s">
+        <v>36</v>
+      </c>
+      <c r="G18" s="3">
+        <f>SUMPRODUCT(F11:F16,G11:G16)/SUM(F11:F14)</f>
+        <v>2.5220000000000002</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DBF20CB-EC62-8543-9C04-FE3F502E9283}">
   <dimension ref="D7:G19"/>
   <sheetViews>
@@ -814,10 +933,10 @@
   </cols>
   <sheetData>
     <row r="7" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="9"/>
+      <c r="E7" s="10"/>
     </row>
     <row r="8" spans="4:7" x14ac:dyDescent="0.2">
       <c r="D8" t="s">

</xml_diff>